<commit_message>
Updates for PreHearingDeposit case creation manually
</commit_message>
<xml_diff>
--- a/src/test/resources/PreHearingDepositData.xlsx
+++ b/src/test/resources/PreHearingDepositData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmet.dede/dev/IntelliJ/et_callbacks/et-ccd-callbacks/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE1F3D9-5812-6942-A854-5954D04953D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A6947-1F33-2642-A22D-0DFD4B870D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43500" yWindow="4760" windowWidth="26440" windowHeight="15440" xr2:uid="{B8523A64-4B85-B14F-8607-0D1E7CC6D2B6}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Case no.</t>
   </si>
@@ -125,28 +125,7 @@
     <t>REFUND UPLOADED</t>
   </si>
   <si>
-    <t>3200954/2008</t>
-  </si>
-  <si>
-    <t>Ms C Mensah-Dapaah</t>
-  </si>
-  <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>000010, 088002, 35897295</t>
-  </si>
-  <si>
-    <t>Kiran</t>
-  </si>
-  <si>
-    <t>TE182000126</t>
-  </si>
-  <si>
-    <t>Royal Mencap Society</t>
-  </si>
-  <si>
-    <t>TE18200618</t>
   </si>
   <si>
     <t>Closed</t>
@@ -155,58 +134,13 @@
     <t>Aberdeen</t>
   </si>
   <si>
-    <t>2600000/2007</t>
-  </si>
-  <si>
-    <t>Mrs O M Adeyemi</t>
-  </si>
-  <si>
-    <t>Drina Tuckett</t>
-  </si>
-  <si>
-    <t>Dr O M Adeyemi</t>
-  </si>
-  <si>
-    <t>ETS-1869-191112-11</t>
-  </si>
-  <si>
     <t>Ashford</t>
-  </si>
-  <si>
-    <t>1701606/2009</t>
-  </si>
-  <si>
-    <t>Mrs A Whitfield</t>
-  </si>
-  <si>
-    <t>013257</t>
-  </si>
-  <si>
-    <t>Peters Langsford Davies Sols</t>
-  </si>
-  <si>
-    <t>TE182000178</t>
-  </si>
-  <si>
-    <t>ETS-1714-160712-13</t>
   </si>
   <si>
     <t>Settled</t>
   </si>
   <si>
     <t>Bedford</t>
-  </si>
-  <si>
-    <t>2201582/2009</t>
-  </si>
-  <si>
-    <t>Mr A Sanni</t>
-  </si>
-  <si>
-    <t>City London Corp</t>
-  </si>
-  <si>
-    <t>ETS-2142-240613-8</t>
   </si>
   <si>
     <t>Struck Out</t>
@@ -228,6 +162,102 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Test Respondent 2</t>
+  </si>
+  <si>
+    <t>Test Respondent 1</t>
+  </si>
+  <si>
+    <t>Test Respondent 3</t>
+  </si>
+  <si>
+    <t>Test Respondent 4</t>
+  </si>
+  <si>
+    <t>2345678/2023</t>
+  </si>
+  <si>
+    <t>3456789/2023</t>
+  </si>
+  <si>
+    <t>1234567/2023</t>
+  </si>
+  <si>
+    <t>8945612/2023</t>
+  </si>
+  <si>
+    <t>123456, 234567, 345678945</t>
+  </si>
+  <si>
+    <t>456789</t>
+  </si>
+  <si>
+    <t>567891</t>
+  </si>
+  <si>
+    <t>894238</t>
+  </si>
+  <si>
+    <t>Test Receiver 1</t>
+  </si>
+  <si>
+    <t>Test Receiver 2</t>
+  </si>
+  <si>
+    <t>Test Receiver 3</t>
+  </si>
+  <si>
+    <t>Test Receiver 4</t>
+  </si>
+  <si>
+    <t>Test Deposit Received From 1</t>
+  </si>
+  <si>
+    <t>Test Deposit Received From 2</t>
+  </si>
+  <si>
+    <t>Test Deposit Received From 3</t>
+  </si>
+  <si>
+    <t>Test Deposit Received From 4</t>
+  </si>
+  <si>
+    <t>Test Comment 1</t>
+  </si>
+  <si>
+    <t>Test Comment 2</t>
+  </si>
+  <si>
+    <t>Test Comment 4</t>
+  </si>
+  <si>
+    <t>Test Comment 3</t>
+  </si>
+  <si>
+    <t>TE123456789</t>
+  </si>
+  <si>
+    <t>TE234567890</t>
+  </si>
+  <si>
+    <t>Test Payee 1</t>
+  </si>
+  <si>
+    <t>Test Payee 2</t>
+  </si>
+  <si>
+    <t>AS123456</t>
+  </si>
+  <si>
+    <t>ATS-1234-121113-11</t>
+  </si>
+  <si>
+    <t>SSS-1111-222222-22</t>
+  </si>
+  <si>
+    <t>DDD-2222-333333-6</t>
   </si>
 </sst>
 </file>
@@ -14807,8 +14837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA58CA0-2F50-0841-AF39-AA9A78A92D3A}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14910,44 +14940,46 @@
     </row>
     <row r="2" spans="1:29" s="43" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="25">
+        <v>44927</v>
+      </c>
+      <c r="D2" s="25">
+        <v>45181</v>
+      </c>
+      <c r="E2" s="26">
+        <v>315</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="25">
-        <v>39709</v>
-      </c>
-      <c r="D2" s="25">
-        <v>39703</v>
-      </c>
-      <c r="E2" s="26">
-        <v>150</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" s="25">
-        <v>41039</v>
+        <v>45056</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="L2" s="29">
-        <v>1768</v>
+        <v>1234</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="N2" s="25">
-        <v>39708</v>
+        <v>45186</v>
       </c>
       <c r="O2" s="31"/>
       <c r="P2" s="32"/>
@@ -14955,35 +14987,35 @@
         <v>5</v>
       </c>
       <c r="R2" s="33">
-        <v>41039</v>
+        <v>45056</v>
       </c>
       <c r="S2" s="34">
         <v>150</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="U2" s="31" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="V2" s="35">
-        <v>41050</v>
+        <v>45067</v>
       </c>
       <c r="W2" s="36"/>
       <c r="X2" s="37" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="38">
         <v>32</v>
       </c>
       <c r="Z2" s="39" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="AA2" s="40">
         <v>10</v>
       </c>
       <c r="AB2" s="41" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="AC2" s="42" t="e">
         <f>VLOOKUP(A2,[1]RefundsYTD!$T$2:$X$997,5,0)</f>
@@ -14992,32 +15024,34 @@
     </row>
     <row r="3" spans="1:29" s="43" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25">
-        <v>40004</v>
+        <v>45117</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="25">
+        <v>45246</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="25">
-        <v>41229</v>
-      </c>
-      <c r="H3" s="44">
-        <v>100154</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="30"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
       <c r="N3" s="25"/>
@@ -15027,17 +15061,17 @@
         <v>5</v>
       </c>
       <c r="R3" s="25">
-        <v>41229</v>
+        <v>45246</v>
       </c>
       <c r="S3" s="27">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="T3" s="29"/>
       <c r="U3" s="29" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="V3" s="45">
-        <v>41233</v>
+        <v>45250</v>
       </c>
       <c r="W3" s="29"/>
       <c r="X3" s="37" t="s">
@@ -15047,13 +15081,13 @@
         <v>26</v>
       </c>
       <c r="Z3" s="39" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AA3" s="40">
         <v>11</v>
       </c>
       <c r="AB3" s="41" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="AC3" s="42" t="e">
         <f>VLOOKUP(A3,[1]RefundsYTD!$T$2:$X$997,5,0)</f>
@@ -15062,44 +15096,46 @@
     </row>
     <row r="4" spans="1:29" s="43" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="25">
-        <v>40093</v>
+        <v>45206</v>
       </c>
       <c r="D4" s="25">
-        <v>40088</v>
+        <v>45201</v>
       </c>
       <c r="E4" s="26">
-        <v>300</v>
+        <v>212</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="25">
-        <v>41096</v>
+        <v>45113</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="L4" s="29">
-        <v>2228</v>
+        <v>2345</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="N4" s="25">
-        <v>40093</v>
+        <v>45206</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="24"/>
@@ -15107,33 +15143,33 @@
         <v>5</v>
       </c>
       <c r="R4" s="25">
-        <v>41096</v>
+        <v>45113</v>
       </c>
       <c r="S4" s="27">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="T4" s="29"/>
       <c r="U4" s="29" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="V4" s="45">
-        <v>41107</v>
+        <v>45124</v>
       </c>
       <c r="W4" s="29"/>
       <c r="X4" s="37" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="38">
         <v>17</v>
       </c>
       <c r="Z4" s="39" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="AA4" s="40">
         <v>12</v>
       </c>
       <c r="AB4" s="41" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="AC4" s="42" t="e">
         <f>VLOOKUP(A4,[1]RefundsYTD!$T$2:$X$997,5,0)</f>
@@ -15142,38 +15178,40 @@
     </row>
     <row r="5" spans="1:29" s="43" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="25">
+        <v>45221</v>
+      </c>
+      <c r="D5" s="25">
+        <v>45201</v>
+      </c>
+      <c r="E5" s="26">
+        <v>495</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="25">
+        <v>45098</v>
+      </c>
+      <c r="H5" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="25">
-        <v>40107</v>
-      </c>
-      <c r="D5" s="25">
-        <v>40088</v>
-      </c>
-      <c r="E5" s="26">
-        <v>500</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="25">
-        <v>41446</v>
-      </c>
-      <c r="H5" s="44">
-        <v>100345</v>
-      </c>
       <c r="I5" s="29" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
-      <c r="K5" s="30"/>
+      <c r="K5" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="L5" s="29">
-        <v>2233</v>
+        <v>3456</v>
       </c>
       <c r="M5" s="29"/>
       <c r="N5" s="25"/>
@@ -15183,35 +15221,35 @@
         <v>5</v>
       </c>
       <c r="R5" s="25">
-        <v>41446</v>
+        <v>45098</v>
       </c>
       <c r="S5" s="27">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="U5" s="29" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="V5" s="45">
-        <v>41450</v>
+        <v>45102</v>
       </c>
       <c r="W5" s="29"/>
       <c r="X5" s="37" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="38">
         <v>22</v>
       </c>
       <c r="Z5" s="39" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="AA5" s="40">
         <v>13</v>
       </c>
       <c r="AB5" s="41" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="AC5" s="42" t="e">
         <f>VLOOKUP(A5,[1]RefundsYTD!$T$2:$X$997,5,0)</f>

</xml_diff>